<commit_message>
Literatura i grafovi fix
</commit_message>
<xml_diff>
--- a/AverageFPS_Results.xlsx
+++ b/AverageFPS_Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>OOP</t>
   </si>
@@ -45,13 +45,22 @@
     <t>EXTREME</t>
   </si>
   <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
     <t>DIFFERENCE</t>
   </si>
   <si>
-    <t>INCREASE IN %</t>
+    <t>Nisko</t>
+  </si>
+  <si>
+    <t>Srednje</t>
+  </si>
+  <si>
+    <t>Visoko</t>
+  </si>
+  <si>
+    <t>Ekstremno</t>
+  </si>
+  <si>
+    <t>Poboljšanje performansa u %</t>
   </si>
 </sst>
 </file>
@@ -267,20 +276,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221218304"/>
-        <c:axId val="221219840"/>
+        <c:axId val="206935168"/>
+        <c:axId val="206936704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221218304"/>
+        <c:axId val="206935168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Izvođenje</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.43851496905401771"/>
+              <c:y val="0.89256926217556143"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221219840"/>
+        <c:crossAx val="206936704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221219840"/>
+        <c:axId val="206936704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -297,11 +333,38 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Prosječan broj osvježavanja po sekundi</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2222227082726833E-2"/>
+              <c:y val="9.9837780694079906E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221218304"/>
+        <c:crossAx val="206935168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -434,20 +497,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221541120"/>
-        <c:axId val="221542656"/>
+        <c:axId val="207253888"/>
+        <c:axId val="207255424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221541120"/>
+        <c:axId val="207253888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Izvođenje</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.43851496905401771"/>
+              <c:y val="0.88793963254593178"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221542656"/>
+        <c:crossAx val="207255424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -455,7 +545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221542656"/>
+        <c:axId val="207255424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="310"/>
@@ -464,11 +554,38 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Prosječan broj osvježavanja po sekundi</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2222227082726833E-2"/>
+              <c:y val="9.1585374744823575E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221541120"/>
+        <c:crossAx val="207253888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -603,20 +720,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221569024"/>
-        <c:axId val="221570560"/>
+        <c:axId val="207281536"/>
+        <c:axId val="207283328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221569024"/>
+        <c:axId val="207281536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Izvođenje</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.41461920384951884"/>
+              <c:y val="0.89719889180519097"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221570560"/>
+        <c:crossAx val="207283328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -624,7 +768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221570560"/>
+        <c:axId val="207283328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="240"/>
@@ -633,11 +777,38 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Prosječan broj ovježavanja po sekundi</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2222222222222223E-2"/>
+              <c:y val="9.0532589676290451E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221569024"/>
+        <c:crossAx val="207281536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -772,20 +943,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221420544"/>
-        <c:axId val="221426432"/>
+        <c:axId val="164207232"/>
+        <c:axId val="164217216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221420544"/>
+        <c:axId val="164207232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Izvođenje</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42017475940507437"/>
+              <c:y val="0.89719889180519097"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221426432"/>
+        <c:crossAx val="164217216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -793,7 +991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221426432"/>
+        <c:axId val="164217216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -802,11 +1000,42 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Prosječan broj</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hr-HR" baseline="0"/>
+                  <a:t> osvježavanja po sekundi</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.5000000000000001E-2"/>
+              <c:y val="9.5208151064450283E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221420544"/>
+        <c:crossAx val="164207232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -898,16 +1127,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>LOW</c:v>
+                  <c:v>Nisko</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MEDIUM</c:v>
+                  <c:v>Srednje</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>HIGH</c:v>
+                  <c:v>Visoko</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EXTREME</c:v>
+                  <c:v>Ekstremno</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -981,16 +1210,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>LOW</c:v>
+                  <c:v>Nisko</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MEDIUM</c:v>
+                  <c:v>Srednje</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>HIGH</c:v>
+                  <c:v>Visoko</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EXTREME</c:v>
+                  <c:v>Ekstremno</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1027,20 +1256,47 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175876736"/>
-        <c:axId val="39978112"/>
+        <c:axId val="163974144"/>
+        <c:axId val="163980032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175876736"/>
+        <c:axId val="163974144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Razina opterećenja</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45659208223972009"/>
+              <c:y val="0.88793963254593178"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39978112"/>
+        <c:crossAx val="163980032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1048,18 +1304,45 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39978112"/>
+        <c:axId val="163980032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Prosječan broj osvježavanja po sekundi</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2222222222222223E-2"/>
+              <c:y val="0.1137266695829688"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175876736"/>
+        <c:crossAx val="163974144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1110,7 +1393,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INCREASE IN %</c:v>
+                  <c:v>Poboljšanje performansa u %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1121,16 +1404,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>LOW</c:v>
+                  <c:v>Nisko</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MEDIUM</c:v>
+                  <c:v>Srednje</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>HIGH</c:v>
+                  <c:v>Visoko</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EXTREME</c:v>
+                  <c:v>Ekstremno</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1168,20 +1451,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163989760"/>
-        <c:axId val="163995648"/>
+        <c:axId val="164025088"/>
+        <c:axId val="164026624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163989760"/>
+        <c:axId val="164025088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Razina opterećenja</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36798687664041996"/>
+              <c:y val="0.89256926217556143"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163995648"/>
+        <c:crossAx val="164026624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1189,18 +1499,38 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163995648"/>
+        <c:axId val="164026624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>Poboljšanje u %</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163989760"/>
+        <c:crossAx val="164025088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1696,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,16 +2289,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2007,21 +2337,21 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>9.4621799999999325</v>
@@ -2038,21 +2368,21 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1">
         <v>1.6</v>

</xml_diff>